<commit_message>
JUnit testing for lookupProduct, lab03
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1346681-3DE2-45FD-AB5D-CAF655458541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A250D5-DA78-4030-B234-DBF4103B79D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="135">
   <si>
     <t>VVSS, Info Romana, 2023-2024</t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t xml:space="preserve">1. La proiectarea TCs se consideră o metodă care poate avea următoarea semnătură: </t>
-  </si>
-  <si>
-    <t>addMovie(String title, String director, int year, List&lt;String&gt; actors, String category, List&lt;String&gt; keywords): void</t>
   </si>
   <si>
     <t>2. Metoda este definită la nivelul repository, service sau ui.</t>
@@ -678,6 +675,12 @@
   </si>
   <si>
     <t>TC9_BVA</t>
+  </si>
+  <si>
+    <t>F01. adăugarea unei piese noi (denumire, numar de bucati, pret, numar minim, numar maxim, id masina);</t>
+  </si>
+  <si>
+    <t>addInhousePart(String name, double price, int inStock, int min, int  max, int partDynamicValue): void</t>
   </si>
 </sst>
 </file>
@@ -1320,7 +1323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1412,6 +1415,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1430,6 +1451,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1491,9 +1518,138 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1502,108 +1658,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1616,57 +1670,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1976,8 +1980,8 @@
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1990,12 +1994,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
       <c r="H1" s="37" t="s">
         <v>1</v>
       </c>
@@ -2003,11 +2007,11 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
@@ -2023,7 +2027,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J4" s="2">
         <v>232</v>
@@ -2034,7 +2038,7 @@
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J5" s="2">
         <v>232</v>
@@ -2046,7 +2050,7 @@
         <v>7</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J6" s="2">
         <v>232</v>
@@ -2102,8 +2106,8 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>14</v>
+      <c r="B16" s="126" t="s">
+        <v>133</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2126,17 +2130,17 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C20" s="33" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2153,7 +2157,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -2170,21 +2174,21 @@
     </row>
     <row r="24" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="34"/>
-      <c r="B24" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
+      <c r="B24" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C26" s="36"/>
@@ -2207,8 +2211,8 @@
   </sheetPr>
   <dimension ref="B1:Q22"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2229,131 +2233,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="60"/>
+      <c r="B3" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="G5" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="G5" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="72"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="G6" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="63" t="s">
+      <c r="H6" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="51" t="s">
+      <c r="I6" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="49" t="s">
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="53"/>
+      <c r="Q6" s="63"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="55" t="s">
-        <v>79</v>
+      <c r="C7" s="65" t="s">
+        <v>78</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="52"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="62"/>
       <c r="I7" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="K7" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="L7" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="N7" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="N7" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="O7" s="50"/>
-      <c r="P7" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q7" s="50"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="60"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="55"/>
+      <c r="C8" s="65"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="107">
+        <v>79</v>
+      </c>
+      <c r="G8" s="39">
         <v>1</v>
       </c>
       <c r="H8" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="22" t="s">
         <v>86</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>87</v>
       </c>
       <c r="J8" s="22">
         <v>2</v>
@@ -2367,36 +2371,36 @@
       <c r="M8" s="22">
         <v>4</v>
       </c>
-      <c r="N8" s="65">
+      <c r="N8" s="53">
         <v>6</v>
       </c>
-      <c r="O8" s="66" t="s">
+      <c r="O8" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="P8" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q8" s="66"/>
+      <c r="Q8" s="54"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="55" t="s">
-        <v>81</v>
+      <c r="C9" s="65" t="s">
+        <v>80</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="10">
         <v>2</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J9" s="22">
         <v>2</v>
@@ -2410,40 +2414,40 @@
       <c r="M9" s="22">
         <v>4</v>
       </c>
-      <c r="N9" s="65">
+      <c r="N9" s="53">
         <v>6</v>
       </c>
-      <c r="O9" s="66" t="s">
-        <v>36</v>
-      </c>
-      <c r="P9" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q9" s="48"/>
+      <c r="O9" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q9" s="58"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="55"/>
+      <c r="C10" s="65"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G10" s="10">
         <v>3</v>
       </c>
-      <c r="H10" s="110" t="s">
-        <v>95</v>
+      <c r="H10" s="40" t="s">
+        <v>94</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J10" s="22">
         <v>2</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L10" s="22">
         <v>3</v>
@@ -2451,31 +2455,31 @@
       <c r="M10" s="22">
         <v>4</v>
       </c>
-      <c r="N10" s="65">
+      <c r="N10" s="53">
         <v>6</v>
       </c>
-      <c r="O10" s="66"/>
-      <c r="P10" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q10" s="48"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q10" s="58"/>
     </row>
     <row r="11" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="E11" s="4"/>
       <c r="G11" s="10">
         <v>4</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I11" s="22">
         <v>123</v>
@@ -2492,25 +2496,25 @@
       <c r="M11" s="22">
         <v>4</v>
       </c>
-      <c r="N11" s="65">
+      <c r="N11" s="53">
         <v>6</v>
       </c>
-      <c r="O11" s="66"/>
-      <c r="P11" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q11" s="48"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q11" s="58"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="55"/>
+      <c r="C12" s="65"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G12" s="107">
+        <v>84</v>
+      </c>
+      <c r="G12" s="39">
         <v>5</v>
       </c>
       <c r="H12" s="22"/>
@@ -2521,17 +2525,17 @@
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
       <c r="O12" s="22"/>
-      <c r="P12" s="65"/>
-      <c r="Q12" s="66"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="54"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="56"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="G13" s="107">
+      <c r="G13" s="39">
         <v>6</v>
       </c>
       <c r="H13" s="22"/>
@@ -2540,19 +2544,19 @@
       <c r="K13" s="22"/>
       <c r="L13" s="22"/>
       <c r="M13" s="22"/>
-      <c r="N13" s="65"/>
-      <c r="O13" s="66"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="66"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="54"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="G14" s="107">
+      <c r="G14" s="39">
         <v>7</v>
       </c>
       <c r="H14" s="22"/>
@@ -2561,21 +2565,21 @@
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
-      <c r="N14" s="108"/>
-      <c r="O14" s="109"/>
-      <c r="P14" s="65"/>
-      <c r="Q14" s="66"/>
+      <c r="N14" s="75"/>
+      <c r="O14" s="76"/>
+      <c r="P14" s="53"/>
+      <c r="Q14" s="54"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="55" t="s">
-        <v>35</v>
+      <c r="C15" s="65" t="s">
+        <v>34</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="G15" s="107">
+      <c r="G15" s="39">
         <v>8</v>
       </c>
       <c r="H15" s="22"/>
@@ -2584,76 +2588,76 @@
       <c r="K15" s="22"/>
       <c r="L15" s="22"/>
       <c r="M15" s="22"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="66"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="66"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="53"/>
+      <c r="Q15" s="54"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="55"/>
+      <c r="C16" s="65"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="G16" s="107"/>
+      <c r="G16" s="39"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
-      <c r="N16" s="65"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="65"/>
-      <c r="Q16" s="66"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="54"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="55" t="s">
-        <v>35</v>
+      <c r="C17" s="65" t="s">
+        <v>34</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="G17" s="107"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
       <c r="L17" s="22"/>
       <c r="M17" s="22"/>
-      <c r="N17" s="65"/>
-      <c r="O17" s="66"/>
-      <c r="P17" s="65"/>
-      <c r="Q17" s="66"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="54"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="54"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="55"/>
+      <c r="C18" s="65"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="G18" s="107"/>
+      <c r="G18" s="39"/>
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
-      <c r="N18" s="65"/>
-      <c r="O18" s="66"/>
-      <c r="P18" s="65"/>
-      <c r="Q18" s="66"/>
+      <c r="N18" s="53"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="54"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="55" t="s">
-        <v>35</v>
+      <c r="C19" s="65" t="s">
+        <v>34</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -2664,25 +2668,25 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="47"/>
-      <c r="Q19" s="48"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="56"/>
+      <c r="P19" s="57"/>
+      <c r="Q19" s="58"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="55"/>
+      <c r="C20" s="65"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
+        <v>38</v>
+      </c>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="41">
@@ -2739,8 +2743,8 @@
   </sheetPr>
   <dimension ref="B1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28:M28"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2764,123 +2768,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="60"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="81" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="62"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="72"/>
     </row>
     <row r="6" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="G6" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="G6" s="112" t="s">
+      <c r="H6" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="112" t="s">
+      <c r="I6" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="112" t="s">
+      <c r="J6" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="113" t="s">
+      <c r="K6" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6" s="79"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="66">
+        <v>1</v>
+      </c>
+      <c r="C7" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="M7" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="N7" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="O7" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="P7" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q7" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="114" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="115"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="115"/>
-      <c r="O6" s="115"/>
-      <c r="P6" s="116"/>
-      <c r="Q6" s="114" t="s">
-        <v>31</v>
-      </c>
-      <c r="R6" s="116"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="56">
-        <v>1</v>
-      </c>
-      <c r="C7" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="R7" s="92"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="86"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="G7" s="117"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="118"/>
-      <c r="K7" s="107" t="s">
-        <v>88</v>
-      </c>
-      <c r="L7" s="107" t="s">
-        <v>113</v>
-      </c>
-      <c r="M7" s="119" t="s">
-        <v>90</v>
-      </c>
-      <c r="N7" s="119" t="s">
-        <v>114</v>
-      </c>
-      <c r="O7" s="107" t="s">
-        <v>92</v>
-      </c>
-      <c r="P7" s="107" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q7" s="120" t="s">
-        <v>47</v>
-      </c>
-      <c r="R7" s="121"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="71"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
@@ -2891,7 +2895,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L8" s="22">
         <v>2</v>
@@ -2908,29 +2912,29 @@
       <c r="P8" s="22">
         <v>6</v>
       </c>
-      <c r="Q8" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="R8" s="66"/>
+      <c r="Q8" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="R8" s="54"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="71"/>
-      <c r="C9" s="73"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G9" s="107">
+        <v>104</v>
+      </c>
+      <c r="G9" s="39">
         <v>2</v>
       </c>
       <c r="H9" s="9">
         <v>2</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L9" s="22">
         <v>2</v>
@@ -2944,21 +2948,21 @@
       <c r="O9" s="22">
         <v>4</v>
       </c>
-      <c r="P9" s="123">
+      <c r="P9" s="44">
         <v>6</v>
       </c>
-      <c r="Q9" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="R9" s="66"/>
+      <c r="Q9" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="R9" s="54"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="71"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="88"/>
       <c r="D10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" s="107">
+        <v>103</v>
+      </c>
+      <c r="G10" s="39">
         <v>3</v>
       </c>
       <c r="H10" s="9">
@@ -2967,7 +2971,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L10" s="22">
         <v>2</v>
@@ -2984,18 +2988,18 @@
       <c r="P10" s="22">
         <v>6</v>
       </c>
-      <c r="Q10" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="R10" s="66"/>
+      <c r="Q10" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="R10" s="54"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="71"/>
-      <c r="C11" s="73"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="88"/>
       <c r="D11" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" s="107">
+        <v>105</v>
+      </c>
+      <c r="G11" s="39">
         <v>4</v>
       </c>
       <c r="H11" s="9">
@@ -3004,7 +3008,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L11" s="22">
         <v>2</v>
@@ -3021,29 +3025,29 @@
       <c r="P11" s="22">
         <v>6</v>
       </c>
-      <c r="Q11" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="R11" s="66"/>
+      <c r="Q11" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" s="54"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="57"/>
-      <c r="C12" s="74"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="107">
+        <v>50</v>
+      </c>
+      <c r="G12" s="39">
         <v>5</v>
       </c>
       <c r="H12" s="9">
         <v>5</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L12" s="22">
         <v>2</v>
@@ -3060,20 +3064,20 @@
       <c r="P12" s="22">
         <v>6</v>
       </c>
-      <c r="Q12" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="R12" s="66"/>
+      <c r="Q12" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="R12" s="54"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="56">
+      <c r="B13" s="66">
         <v>2</v>
       </c>
-      <c r="C13" s="56" t="s">
-        <v>101</v>
+      <c r="C13" s="66" t="s">
+        <v>100</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G13" s="10">
         <v>6</v>
@@ -3083,10 +3087,10 @@
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L13" s="22">
         <v>2</v>
@@ -3103,16 +3107,16 @@
       <c r="P13" s="22">
         <v>6</v>
       </c>
-      <c r="Q13" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="R13" s="66"/>
+      <c r="Q13" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="R13" s="54"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="86"/>
       <c r="D14" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G14" s="10">
         <v>7</v>
@@ -3121,11 +3125,11 @@
         <v>7</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L14" s="22">
         <v>2</v>
@@ -3142,18 +3146,18 @@
       <c r="P14" s="22">
         <v>6</v>
       </c>
-      <c r="Q14" s="65" t="s">
-        <v>118</v>
-      </c>
-      <c r="R14" s="66"/>
+      <c r="Q14" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="R14" s="54"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="86"/>
       <c r="D15" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" s="107">
+        <v>108</v>
+      </c>
+      <c r="G15" s="39">
         <v>8</v>
       </c>
       <c r="H15" s="9">
@@ -3162,7 +3166,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L15" s="22">
         <v>2</v>
@@ -3179,18 +3183,18 @@
       <c r="P15" s="22">
         <v>6</v>
       </c>
-      <c r="Q15" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="R15" s="66"/>
+      <c r="Q15" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="R15" s="54"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
       <c r="D16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G16" s="107">
+        <v>109</v>
+      </c>
+      <c r="G16" s="39">
         <v>9</v>
       </c>
       <c r="H16" s="9">
@@ -3199,7 +3203,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L16" s="22">
         <v>2</v>
@@ -3216,27 +3220,27 @@
       <c r="P16" s="22">
         <v>6</v>
       </c>
-      <c r="Q16" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="R16" s="66"/>
+      <c r="Q16" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="R16" s="54"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
       <c r="D17" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="107">
+        <v>110</v>
+      </c>
+      <c r="G17" s="39">
         <v>10</v>
       </c>
-      <c r="H17" s="111">
+      <c r="H17" s="41">
         <v>10</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L17" s="22">
         <v>2</v>
@@ -3253,18 +3257,18 @@
       <c r="P17" s="22">
         <v>6</v>
       </c>
-      <c r="Q17" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="R17" s="66"/>
+      <c r="Q17" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="R17" s="54"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" s="107">
+        <v>111</v>
+      </c>
+      <c r="G18" s="39">
         <v>11</v>
       </c>
       <c r="H18" s="9">
@@ -3273,7 +3277,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L18" s="22">
         <v>2</v>
@@ -3290,16 +3294,16 @@
       <c r="P18" s="22">
         <v>6</v>
       </c>
-      <c r="Q18" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="R18" s="66"/>
+      <c r="Q18" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="R18" s="54"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="56">
+      <c r="B19" s="66">
         <v>3</v>
       </c>
-      <c r="C19" s="72"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="2"/>
       <c r="G19" s="10">
         <v>12</v>
@@ -3310,7 +3314,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L19" s="22">
         <v>2</v>
@@ -3327,16 +3331,16 @@
       <c r="P19" s="22">
         <v>6</v>
       </c>
-      <c r="Q19" s="65" t="s">
-        <v>119</v>
-      </c>
-      <c r="R19" s="66"/>
+      <c r="Q19" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="R19" s="54"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="71"/>
-      <c r="C20" s="73"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="88"/>
       <c r="D20" s="2"/>
-      <c r="G20" s="107">
+      <c r="G20" s="39">
         <v>13</v>
       </c>
       <c r="H20" s="9"/>
@@ -3348,14 +3352,14 @@
       <c r="N20" s="22"/>
       <c r="O20" s="22"/>
       <c r="P20" s="22"/>
-      <c r="Q20" s="65"/>
-      <c r="R20" s="66"/>
+      <c r="Q20" s="53"/>
+      <c r="R20" s="54"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="71"/>
-      <c r="C21" s="73"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="88"/>
       <c r="D21" s="2"/>
-      <c r="G21" s="107">
+      <c r="G21" s="39">
         <v>14</v>
       </c>
       <c r="H21" s="9"/>
@@ -3367,14 +3371,14 @@
       <c r="N21" s="22"/>
       <c r="O21" s="22"/>
       <c r="P21" s="22"/>
-      <c r="Q21" s="65"/>
-      <c r="R21" s="66"/>
+      <c r="Q21" s="53"/>
+      <c r="R21" s="54"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="71"/>
-      <c r="C22" s="73"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="88"/>
       <c r="D22" s="2"/>
-      <c r="G22" s="107">
+      <c r="G22" s="39">
         <v>15</v>
       </c>
       <c r="H22" s="9"/>
@@ -3386,14 +3390,14 @@
       <c r="N22" s="22"/>
       <c r="O22" s="22"/>
       <c r="P22" s="22"/>
-      <c r="Q22" s="65"/>
-      <c r="R22" s="66"/>
+      <c r="Q22" s="53"/>
+      <c r="R22" s="54"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B23" s="71"/>
-      <c r="C23" s="73"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="88"/>
       <c r="D23" s="2"/>
-      <c r="G23" s="107">
+      <c r="G23" s="39">
         <v>16</v>
       </c>
       <c r="H23" s="9"/>
@@ -3405,14 +3409,14 @@
       <c r="N23" s="22"/>
       <c r="O23" s="22"/>
       <c r="P23" s="22"/>
-      <c r="Q23" s="65"/>
-      <c r="R23" s="66"/>
+      <c r="Q23" s="53"/>
+      <c r="R23" s="54"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B24" s="57"/>
-      <c r="C24" s="74"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="89"/>
       <c r="D24" s="2"/>
-      <c r="G24" s="107">
+      <c r="G24" s="39">
         <v>17</v>
       </c>
       <c r="H24" s="9"/>
@@ -3424,20 +3428,20 @@
       <c r="N24" s="22"/>
       <c r="O24" s="22"/>
       <c r="P24" s="22"/>
-      <c r="Q24" s="65"/>
-      <c r="R24" s="66"/>
+      <c r="Q24" s="53"/>
+      <c r="R24" s="54"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B25" s="56">
+      <c r="B25" s="66">
         <v>4</v>
       </c>
-      <c r="C25" s="72" t="s">
-        <v>35</v>
+      <c r="C25" s="87" t="s">
+        <v>34</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="107">
+        <v>34</v>
+      </c>
+      <c r="G25" s="39">
         <v>18</v>
       </c>
       <c r="H25" s="9"/>
@@ -3449,68 +3453,68 @@
       <c r="N25" s="22"/>
       <c r="O25" s="22"/>
       <c r="P25" s="22"/>
-      <c r="Q25" s="65"/>
-      <c r="R25" s="66"/>
+      <c r="Q25" s="53"/>
+      <c r="R25" s="54"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B26" s="71"/>
-      <c r="C26" s="73"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="88"/>
       <c r="D26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="122"/>
-      <c r="H26" s="122"/>
-      <c r="I26" s="122"/>
-      <c r="J26" s="122"/>
-      <c r="K26" s="122"/>
-      <c r="L26" s="122"/>
-      <c r="M26" s="122"/>
-      <c r="N26" s="122"/>
-      <c r="O26" s="122"/>
-      <c r="P26" s="122"/>
-      <c r="Q26" s="122"/>
-      <c r="R26" s="122"/>
+        <v>34</v>
+      </c>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="71"/>
-      <c r="C27" s="73"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="88"/>
       <c r="D27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B28" s="71"/>
-      <c r="C28" s="73"/>
+      <c r="B28" s="86"/>
+      <c r="C28" s="88"/>
       <c r="D28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="69"/>
+        <v>34</v>
+      </c>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="80"/>
+      <c r="M28" s="80"/>
       <c r="N28" s="29"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B29" s="71"/>
-      <c r="C29" s="73"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="88"/>
       <c r="D29" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I29" s="75"/>
-      <c r="J29" s="75"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="75"/>
-      <c r="M29" s="75"/>
+        <v>34</v>
+      </c>
+      <c r="I29" s="90"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="90"/>
       <c r="N29" s="30"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B30" s="57"/>
-      <c r="C30" s="74"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="89"/>
       <c r="D30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3570,7 +3574,7 @@
   <dimension ref="B1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3586,127 +3590,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="125" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="125"/>
+      <c r="N3" s="125"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="106"/>
-      <c r="L3" s="106"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="106"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="63" t="s">
+      <c r="C4" s="123" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="D4" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="E4" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="F4" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="63"/>
+    </row>
+    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="104"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="116" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="117"/>
+      <c r="M5" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="F4" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="53"/>
-    </row>
-    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="92"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="K5" s="99" t="s">
-        <v>93</v>
-      </c>
-      <c r="L5" s="100"/>
-      <c r="M5" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
         <v>1</v>
       </c>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="102" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>61</v>
-      </c>
       <c r="E6" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="125" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" s="125">
+        <v>35</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="46">
         <v>2</v>
       </c>
-      <c r="H6" s="125">
+      <c r="H6" s="46">
         <v>100</v>
       </c>
-      <c r="I6" s="125">
+      <c r="I6" s="46">
         <v>3</v>
       </c>
-      <c r="J6" s="125">
+      <c r="J6" s="46">
         <v>4</v>
       </c>
-      <c r="K6" s="101">
+      <c r="K6" s="118">
         <v>6</v>
       </c>
-      <c r="L6" s="102" t="s">
+      <c r="L6" s="119" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="125" t="s">
-        <v>34</v>
-      </c>
       <c r="N6" s="38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -3714,37 +3718,37 @@
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="90"/>
+      <c r="C7" s="102"/>
       <c r="D7" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="124" t="s">
-        <v>96</v>
-      </c>
-      <c r="G7" s="124">
+        <v>35</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="45">
         <v>2</v>
       </c>
-      <c r="H7" s="124">
+      <c r="H7" s="45">
         <v>-100</v>
       </c>
-      <c r="I7" s="124">
+      <c r="I7" s="45">
         <v>3</v>
       </c>
-      <c r="J7" s="124">
+      <c r="J7" s="45">
         <v>4</v>
       </c>
-      <c r="K7" s="67">
+      <c r="K7" s="120">
         <v>6</v>
       </c>
-      <c r="L7" s="68"/>
-      <c r="M7" s="124" t="s">
-        <v>126</v>
+      <c r="L7" s="121"/>
+      <c r="M7" s="45" t="s">
+        <v>125</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -3752,37 +3756,37 @@
         <f t="shared" ref="B8:B13" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="90"/>
+      <c r="C8" s="102"/>
       <c r="D8" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="124" t="s">
-        <v>97</v>
-      </c>
-      <c r="G8" s="124">
+        <v>35</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="45">
         <v>2</v>
       </c>
-      <c r="H8" s="124" t="s">
-        <v>125</v>
-      </c>
-      <c r="I8" s="124">
+      <c r="H8" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" s="45">
         <v>3</v>
       </c>
-      <c r="J8" s="124">
+      <c r="J8" s="45">
         <v>4</v>
       </c>
-      <c r="K8" s="67">
+      <c r="K8" s="120">
         <v>6</v>
       </c>
-      <c r="L8" s="68"/>
-      <c r="M8" s="124" t="s">
-        <v>127</v>
+      <c r="L8" s="121"/>
+      <c r="M8" s="45" t="s">
+        <v>126</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
@@ -3790,9 +3794,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="90"/>
+      <c r="C9" s="102"/>
       <c r="D9" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12">
@@ -3810,15 +3814,15 @@
       <c r="J9" s="12">
         <v>4</v>
       </c>
-      <c r="K9" s="49">
+      <c r="K9" s="59">
         <v>6</v>
       </c>
-      <c r="L9" s="50"/>
+      <c r="L9" s="60"/>
       <c r="M9" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -3826,37 +3830,37 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="90"/>
+      <c r="C10" s="102"/>
       <c r="D10" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="F10" s="124" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="124">
+      <c r="G10" s="45">
         <v>2</v>
       </c>
-      <c r="H10" s="124">
+      <c r="H10" s="45">
         <v>100</v>
       </c>
-      <c r="I10" s="124">
+      <c r="I10" s="45">
         <v>3</v>
       </c>
-      <c r="J10" s="124">
+      <c r="J10" s="45">
         <v>4</v>
       </c>
-      <c r="K10" s="67">
+      <c r="K10" s="120">
         <v>6</v>
       </c>
-      <c r="L10" s="68"/>
-      <c r="M10" s="124" t="s">
-        <v>117</v>
+      <c r="L10" s="121"/>
+      <c r="M10" s="45" t="s">
+        <v>116</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -3864,37 +3868,37 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="90"/>
+      <c r="C11" s="102"/>
       <c r="D11" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="124" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="124">
+        <v>62</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="45">
         <v>2</v>
       </c>
-      <c r="H11" s="124">
+      <c r="H11" s="45">
         <v>100</v>
       </c>
-      <c r="I11" s="124">
+      <c r="I11" s="45">
         <v>3</v>
       </c>
-      <c r="J11" s="124">
+      <c r="J11" s="45">
         <v>4</v>
       </c>
-      <c r="K11" s="67">
+      <c r="K11" s="120">
         <v>6</v>
       </c>
-      <c r="L11" s="68"/>
-      <c r="M11" s="124" t="s">
-        <v>34</v>
+      <c r="L11" s="121"/>
+      <c r="M11" s="45" t="s">
+        <v>33</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -3902,37 +3906,37 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="90"/>
+      <c r="C12" s="102"/>
       <c r="D12" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="45">
+        <v>2</v>
+      </c>
+      <c r="H12" s="45">
+        <v>0</v>
+      </c>
+      <c r="I12" s="45">
+        <v>3</v>
+      </c>
+      <c r="J12" s="45">
+        <v>4</v>
+      </c>
+      <c r="K12" s="120">
+        <v>6</v>
+      </c>
+      <c r="L12" s="121"/>
+      <c r="M12" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="F12" s="124" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="124">
-        <v>2</v>
-      </c>
-      <c r="H12" s="124">
-        <v>0</v>
-      </c>
-      <c r="I12" s="124">
-        <v>3</v>
-      </c>
-      <c r="J12" s="124">
-        <v>4</v>
-      </c>
-      <c r="K12" s="67">
-        <v>6</v>
-      </c>
-      <c r="L12" s="68"/>
-      <c r="M12" s="124" t="s">
-        <v>132</v>
-      </c>
       <c r="N12" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3940,15 +3944,15 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="91"/>
+      <c r="C13" s="103"/>
       <c r="D13" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" s="15">
         <v>2</v>
@@ -3962,15 +3966,15 @@
       <c r="J13" s="15">
         <v>4</v>
       </c>
-      <c r="K13" s="99">
+      <c r="K13" s="116">
         <v>6</v>
       </c>
-      <c r="L13" s="100"/>
+      <c r="L13" s="117"/>
       <c r="M13" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N13" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -3990,7 +3994,7 @@
     </row>
     <row r="15" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="17"/>
@@ -4000,102 +4004,102 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
+      <c r="K15" s="101"/>
+      <c r="L15" s="101"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="78" t="s">
+      <c r="C17" s="95" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="97"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="25" t="s">
+      <c r="H17" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="78" t="s">
+      <c r="I17" s="96"/>
+      <c r="J17" s="97"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="79"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="81"/>
-      <c r="M17" s="78" t="s">
+      <c r="N17" s="96"/>
+      <c r="O17" s="97"/>
+      <c r="P17" s="98"/>
+    </row>
+    <row r="18" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="109" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="N17" s="79"/>
-      <c r="O17" s="80"/>
-      <c r="P17" s="81"/>
-    </row>
-    <row r="18" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="97" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="98" t="s">
+      <c r="D18" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="76" t="s">
+      <c r="E18" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="76" t="s">
+      <c r="F18" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="77" t="s">
+      <c r="G18" s="115" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="88" t="s">
+      <c r="H18" s="111" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="84" t="s">
-        <v>74</v>
-      </c>
-      <c r="I18" s="85"/>
-      <c r="J18" s="76" t="s">
+      <c r="I18" s="112"/>
+      <c r="J18" s="94" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="K18" s="76" t="s">
+      <c r="L18" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="L18" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="M18" s="82" t="s">
-        <v>74</v>
-      </c>
-      <c r="N18" s="76" t="s">
+      <c r="M18" s="99" t="s">
+        <v>73</v>
+      </c>
+      <c r="N18" s="94" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="O18" s="76" t="s">
+      <c r="P18" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="P18" s="77" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="97"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="77"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="76"/>
-      <c r="K19" s="76"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="83"/>
-      <c r="N19" s="76"/>
-      <c r="O19" s="76"/>
-      <c r="P19" s="77"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="115"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="114"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="94"/>
+      <c r="L19" s="93"/>
+      <c r="M19" s="100"/>
+      <c r="N19" s="94"/>
+      <c r="O19" s="94"/>
+      <c r="P19" s="93"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="24">
         <v>8</v>
@@ -4112,10 +4116,10 @@
       <c r="G20" s="32">
         <v>4</v>
       </c>
-      <c r="H20" s="95" t="s">
-        <v>129</v>
-      </c>
-      <c r="I20" s="96"/>
+      <c r="H20" s="107" t="s">
+        <v>128</v>
+      </c>
+      <c r="I20" s="108"/>
       <c r="J20" s="2">
         <v>4</v>
       </c>
@@ -4126,13 +4130,13 @@
         <v>0</v>
       </c>
       <c r="M20" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N20" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O20" s="26">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="P20" s="27">
         <v>0</v>
@@ -4188,12 +4192,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5F472198D7887469049920058585067" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e76e8f6ca957e849a493f1baa4f4bb7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c46c0853-0d59-45c6-b517-3e25eac8cdf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ddeb00cc2097713d6f56fe4f26be38f" ns2:_="">
     <xsd:import namespace="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
@@ -4337,7 +4335,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4346,16 +4344,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153A5999-B236-48B1-944C-C5EB94545735}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4373,10 +4368,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>